<commit_message>
new models for testing
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\hackathon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75B3D269-24BD-422F-A86C-11D9B6585E26}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F11BF7B4-D6E4-444D-9FB8-1085CFCEF332}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4512" yWindow="3396" windowWidth="17280" windowHeight="8964" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="0 hourly" sheetId="3" r:id="rId1"/>
@@ -420,9 +420,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L721"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
final changes to task 1
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\hackathon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F11BF7B4-D6E4-444D-9FB8-1085CFCEF332}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{908B7BCC-8C45-4A03-83F8-9E44B36B11BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4512" yWindow="3396" windowWidth="17280" windowHeight="8964" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="0 hourly" sheetId="3" r:id="rId1"/>
@@ -54,9 +54,6 @@
     <t>Pressure</t>
   </si>
   <si>
-    <t>Windspeedm/s</t>
-  </si>
-  <si>
     <t>WindDirection</t>
   </si>
   <si>
@@ -64,6 +61,9 @@
   </si>
   <si>
     <t>Temperature</t>
+  </si>
+  <si>
+    <t>WindSpeed</t>
   </si>
 </sst>
 </file>
@@ -420,7 +420,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L721"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
@@ -433,7 +435,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -457,13 +459,13 @@
         <v>7</v>
       </c>
       <c r="J1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>9</v>
-      </c>
-      <c r="L1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>